<commit_message>
Done, under development inpatient certificate
</commit_message>
<xml_diff>
--- a/public/excel/SUMMARY_TEMPLATE.xlsx
+++ b/public/excel/SUMMARY_TEMPLATE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\projects\qrcode-tracker\public\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D649F6C-5CF6-48BE-92B5-ABC0A00B39D2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D507504-8837-4C9E-978C-558CDFB36FB3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{73DADEC1-6CF2-4CD0-A71F-0005749F04E8}"/>
   </bookViews>
@@ -69,7 +69,7 @@
     <t>RECEIVED BY</t>
   </si>
   <si>
-    <t>RELEASED BY</t>
+    <t>RELEASED/CANCELLED BY</t>
   </si>
 </sst>
 </file>
@@ -470,7 +470,7 @@
   <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>